<commit_message>
Modification des fichier excel Raey
</commit_message>
<xml_diff>
--- a/Donnee/Arc/Arc.xlsx
+++ b/Donnee/Arc/Arc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\assef\OneDrive\Bureau\1HEIG\semetre 2\VisualDonne\Projet\Donnee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\assef\OneDrive\Bureau\1HEIG\semetre 2\VisualDonne\Projet\Site\Donnee\Arc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DA7991F-8D4C-411D-8CCE-1E65A429D9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71517A1-EDE3-40F8-A91A-2BF7D984470A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10308" yWindow="1488" windowWidth="14256" windowHeight="12528" xr2:uid="{F3C43482-C596-48FB-A295-3B40618EB8EC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F3C43482-C596-48FB-A295-3B40618EB8EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>East Blue</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>L'arc où Luffy et son équipage affrontent Arlong et sa bande de pirates poissons sur l'île de Nami, qui a été forcée de les aider.</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>Arc</t>
@@ -504,121 +501,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A1139B6-78EB-45B3-96CA-1B788829EFB1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:2" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:2" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:2" ht="138.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:2" ht="193.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:2" ht="152.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="180" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:2" ht="180" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:2" ht="166.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>